<commit_message>
Más mediciones de temperatura
</commit_message>
<xml_diff>
--- a/Pruebas Experimentales/Prueba Temperatura/Prueba 10C/PRUEBA_TEMPERATURA_23_10C.xlsx
+++ b/Pruebas Experimentales/Prueba Temperatura/Prueba 10C/PRUEBA_TEMPERATURA_23_10C.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Datos crudos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Timestamp</t>
   </si>
@@ -73,106 +73,130 @@
     <t>Temperature</t>
   </si>
   <si>
-    <t>2023-12-11 06:02:19</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:03:21</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:04:23</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:05:25</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:06:27</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:07:29</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:08:32</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:09:34</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:10:36</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:11:38</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:12:40</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:13:42</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:14:45</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:15:47</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:16:49</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:17:51</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:18:53</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:19:56</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:20:58</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:22:00</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:23:02</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:24:04</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:25:06</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:26:09</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:27:11</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:28:13</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:29:15</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:30:17</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:31:20</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:32:22</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:33:24</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:34:26</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:35:28</t>
-  </si>
-  <si>
-    <t>2023-12-11 06:36:30</t>
+    <t>2023-12-11 22:57:25</t>
+  </si>
+  <si>
+    <t>2023-12-11 22:58:27</t>
+  </si>
+  <si>
+    <t>2023-12-11 22:59:29</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:00:32</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:01:34</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:02:37</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:03:39</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:04:41</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:05:44</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:06:46</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:07:49</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:08:51</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:09:53</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:10:56</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:11:58</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:13:01</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:14:03</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:15:06</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:16:08</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:17:10</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:18:13</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:19:15</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:20:18</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:21:20</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:22:22</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:23:25</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:24:27</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:25:30</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:26:32</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:27:35</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:28:37</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:29:39</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:30:42</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:31:44</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:32:47</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:33:49</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:34:51</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:35:54</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:36:56</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:37:59</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:39:01</t>
+  </si>
+  <si>
+    <t>2023-12-11 23:40:03</t>
   </si>
 </sst>
 </file>
@@ -839,111 +863,135 @@
           </c:trendline>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos crudos'!$E$2:$E$35</c:f>
+              <c:f>'Datos crudos'!$E$2:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>22.526223776223699</c:v>
+                  <c:v>23.181818181818102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.5594405594405</c:v>
+                  <c:v>21.477272727272702</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>20.034965034965001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.641608391608401</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>18.986013986014001</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>17.937062937062901</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.756993006993</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>18.330419580419498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.543706293706201</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.281468531468501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.019230769230699</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.494755244755201</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.232517482517402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.9702797202797</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.1013986013986</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.9702797202797</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.7080419580419</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.839160839160799</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15.4458041958042</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.4458041958042</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>15.576923076923</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="19">
+                  <c:v>15.576923076923</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.314685314685301</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.314685314685301</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>15.1835664335664</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.921328671328601</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14.659090909090899</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.0034965034965</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14.0034965034965</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13.741258741258701</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.741258741258701</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13.479020979021</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>13.479020979021</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>13.479020979021</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>13.3479020979021</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13.6101398601398</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>13.216783216783201</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>13.216783216783201</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>13.479020979021</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>13.479020979021</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>13.479020979021</c:v>
-                </c:pt>
                 <c:pt idx="23">
-                  <c:v>13.3479020979021</c:v>
+                  <c:v>15.314685314685301</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13.216783216783201</c:v>
+                  <c:v>15.314685314685301</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13.3479020979021</c:v>
+                  <c:v>15.0524475524475</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13.479020979021</c:v>
+                  <c:v>15.1835664335664</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13.3479020979021</c:v>
+                  <c:v>15.1835664335664</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13.479020979021</c:v>
+                  <c:v>15.314685314685301</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13.3479020979021</c:v>
+                  <c:v>15.1835664335664</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13.479020979021</c:v>
+                  <c:v>15.314685314685301</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>14.3968531468531</c:v>
+                  <c:v>15.1835664335664</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>17.805944055944</c:v>
+                  <c:v>15.1835664335664</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>18.8548951048951</c:v>
+                  <c:v>15.4458041958042</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15.314685314685301</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15.1835664335664</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15.314685314685301</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>15.1835664335664</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15.314685314685301</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15.314685314685301</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15.314685314685301</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>15.0524475524475</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1200,37 +1248,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>13.479020979021</c:v>
+                  <c:v>15.1835664335664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.479020979021</c:v>
+                  <c:v>15.1835664335664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.479020979021</c:v>
+                  <c:v>15.4458041958042</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.3479020979021</c:v>
+                  <c:v>15.314685314685301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.216783216783201</c:v>
+                  <c:v>15.1835664335664</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.3479020979021</c:v>
+                  <c:v>15.314685314685301</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.479020979021</c:v>
+                  <c:v>15.1835664335664</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.3479020979021</c:v>
+                  <c:v>15.314685314685301</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.479020979021</c:v>
+                  <c:v>15.314685314685301</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.3479020979021</c:v>
+                  <c:v>15.314685314685301</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.479020979021</c:v>
+                  <c:v>15.0524475524475</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1327,10 +1375,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>13.40750158931978</c:v>
+                  <c:v>15.255085823267619</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.40750158931978</c:v>
+                  <c:v>15.255085823267619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3052,10 +3100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3101,17 +3149,17 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>22.526223776223699</v>
+        <v>23.181818181818102</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
       <c r="H2">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I2" s="4">
         <f>INDEX(C:C,H2)-C2</f>
-        <v>9.3518518551718444E-3</v>
+        <v>4.3287037042318843E-3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3128,14 +3176,14 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>20.5594405594405</v>
+        <v>21.477272727272702</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
       </c>
       <c r="H3">
-        <f>COUNT(E:E)-3</f>
-        <v>31</v>
+        <f>COUNT(E:E)</f>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3152,7 +3200,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>18.986013986014001</v>
+        <v>20.034965034965001</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3169,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>17.937062937062901</v>
+        <v>19.641608391608401</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3186,7 +3234,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>16.756993006993</v>
+        <v>18.986013986014001</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -3203,7 +3251,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>15.576923076923</v>
+        <v>18.330419580419498</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -3220,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="3">
-        <v>15.1835664335664</v>
+        <v>17.543706293706201</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3237,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>14.921328671328601</v>
+        <v>17.281468531468501</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -3254,7 +3302,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>14.659090909090899</v>
+        <v>17.019230769230699</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -3271,7 +3319,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>14.0034965034965</v>
+        <v>16.494755244755201</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -3288,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>14.0034965034965</v>
+        <v>16.232517482517402</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -3305,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>13.741258741258701</v>
+        <v>15.9702797202797</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -3322,7 +3370,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>13.741258741258701</v>
+        <v>16.1013986013986</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -3339,7 +3387,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>13.479020979021</v>
+        <v>15.9702797202797</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -3356,7 +3404,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>13.479020979021</v>
+        <v>15.7080419580419</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -3373,7 +3421,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>13.479020979021</v>
+        <v>15.839160839160799</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -3390,7 +3438,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>13.3479020979021</v>
+        <v>15.4458041958042</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3407,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>13.6101398601398</v>
+        <v>15.4458041958042</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -3424,7 +3472,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>13.216783216783201</v>
+        <v>15.576923076923</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -3441,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>13.216783216783201</v>
+        <v>15.576923076923</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -3458,7 +3506,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>13.479020979021</v>
+        <v>15.314685314685301</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -3475,7 +3523,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>13.479020979021</v>
+        <v>15.314685314685301</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -3492,7 +3540,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>13.479020979021</v>
+        <v>15.1835664335664</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -3509,7 +3557,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>13.3479020979021</v>
+        <v>15.314685314685301</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -3526,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>13.216783216783201</v>
+        <v>15.314685314685301</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -3543,7 +3591,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>13.3479020979021</v>
+        <v>15.0524475524475</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -3560,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>13.479020979021</v>
+        <v>15.1835664335664</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -3577,7 +3625,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>13.3479020979021</v>
+        <v>15.1835664335664</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -3594,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>13.479020979021</v>
+        <v>15.314685314685301</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -3611,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>13.3479020979021</v>
+        <v>15.1835664335664</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -3628,7 +3676,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>13.479020979021</v>
+        <v>15.314685314685301</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -3645,7 +3693,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>14.3968531468531</v>
+        <v>15.1835664335664</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -3662,7 +3710,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>17.805944055944</v>
+        <v>15.1835664335664</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -3679,7 +3727,143 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>18.8548951048951</v>
+        <v>15.4458041958042</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>23</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>15.314685314685301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>15.1835664335664</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>23</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>15.314685314685301</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>23</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>15.1835664335664</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>23</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>15.314685314685301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>23</v>
+      </c>
+      <c r="B41">
+        <v>10</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>15.314685314685301</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>23</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>15.314685314685301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>23</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>15.0524475524475</v>
       </c>
     </row>
   </sheetData>
@@ -3692,8 +3876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3718,45 +3902,45 @@
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A2)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:23:02</v>
+        <v>2023-12-11 23:29:39</v>
       </c>
       <c r="B2">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A2)-ROW($A$2)-9),"")</f>
-        <v>13.479020979021</v>
+        <v>15.1835664335664</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <f>AVERAGE(B:B)</f>
-        <v>13.40750158931978</v>
+        <v>15.255085823267619</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A3)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:24:04</v>
+        <v>2023-12-11 23:30:42</v>
       </c>
       <c r="B3">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A3)-ROW($A$2)-9),"")</f>
-        <v>13.479020979021</v>
+        <v>15.1835664335664</v>
       </c>
       <c r="D3">
         <v>11</v>
       </c>
       <c r="E3">
         <f>AVERAGE(B:B)</f>
-        <v>13.40750158931978</v>
+        <v>15.255085823267619</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A4)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:25:06</v>
+        <v>2023-12-11 23:31:44</v>
       </c>
       <c r="B4">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A4)-ROW($A$2)-9),"")</f>
-        <v>13.479020979021</v>
+        <v>15.4458041958042</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -3765,35 +3949,35 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A5)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:26:09</v>
+        <v>2023-12-11 23:32:47</v>
       </c>
       <c r="B5">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A5)-ROW($A$2)-9),"")</f>
-        <v>13.3479020979021</v>
+        <v>15.314685314685301</v>
       </c>
       <c r="E5">
         <f>_xlfn.STDEV.S(B:B)</f>
-        <v>9.015100318432144E-2</v>
+        <v>0.10754364496479615</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A6)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:27:11</v>
+        <v>2023-12-11 23:33:49</v>
       </c>
       <c r="B6">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A6)-ROW($A$2)-9),"")</f>
-        <v>13.216783216783201</v>
+        <v>15.1835664335664</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A7)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:28:13</v>
+        <v>2023-12-11 23:34:51</v>
       </c>
       <c r="B7">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A7)-ROW($A$2)-9),"")</f>
-        <v>13.3479020979021</v>
+        <v>15.314685314685301</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>7</v>
@@ -3802,36 +3986,36 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A8)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:29:15</v>
+        <v>2023-12-11 23:35:54</v>
       </c>
       <c r="B8">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A8)-ROW($A$2)-9),"")</f>
-        <v>13.479020979021</v>
+        <v>15.1835664335664</v>
       </c>
       <c r="E8">
         <f>MAX(B:B)</f>
-        <v>13.479020979021</v>
+        <v>15.4458041958042</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A9)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:30:17</v>
+        <v>2023-12-11 23:36:56</v>
       </c>
       <c r="B9">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A9)-ROW($A$2)-9),"")</f>
-        <v>13.3479020979021</v>
+        <v>15.314685314685301</v>
       </c>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A10)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:31:20</v>
+        <v>2023-12-11 23:37:59</v>
       </c>
       <c r="B10">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A10)-ROW($A$2)-9),"")</f>
-        <v>13.479020979021</v>
+        <v>15.314685314685301</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
@@ -3840,25 +4024,25 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A11)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:32:22</v>
+        <v>2023-12-11 23:39:01</v>
       </c>
       <c r="B11">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A11)-ROW($A$2)-9),"")</f>
-        <v>13.3479020979021</v>
+        <v>15.314685314685301</v>
       </c>
       <c r="E11">
         <f>MIN(B:B)</f>
-        <v>13.216783216783201</v>
+        <v>15.0524475524475</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IFERROR(INDEX('Datos crudos'!C:C,'Datos crudos'!$H$3+ROW($A12)-ROW($A$2)-9),"")</f>
-        <v>2023-12-11 06:33:24</v>
+        <v>2023-12-11 23:40:03</v>
       </c>
       <c r="B12">
         <f>IFERROR(INDEX('Datos crudos'!E:E,'Datos crudos'!$H$3+ROW($A12)-ROW($A$2)-9),"")</f>
-        <v>13.479020979021</v>
+        <v>15.0524475524475</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>